<commit_message>
update pictures in table
</commit_message>
<xml_diff>
--- a/DataSet.xlsx
+++ b/DataSet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="269">
   <si>
     <t>אבוקדו</t>
   </si>
@@ -652,6 +652,177 @@
   </si>
   <si>
     <t>שהחיינו</t>
+  </si>
+  <si>
+    <t>prichiyot</t>
+  </si>
+  <si>
+    <t>katsefet</t>
+  </si>
+  <si>
+    <t>artik.jpg</t>
+  </si>
+  <si>
+    <t>cofee.jpg</t>
+  </si>
+  <si>
+    <t>falafel.jpg</t>
+  </si>
+  <si>
+    <t>fixtuk.jpg</t>
+  </si>
+  <si>
+    <t>kakaomashke.jpg</t>
+  </si>
+  <si>
+    <t>kinamon.jpg</t>
+  </si>
+  <si>
+    <t>kishu.jpg</t>
+  </si>
+  <si>
+    <t>klementina.jpg</t>
+  </si>
+  <si>
+    <t>kneydalach.jpg</t>
+  </si>
+  <si>
+    <t>kokus.jpg</t>
+  </si>
+  <si>
+    <t>kornflexe.jpg</t>
+  </si>
+  <si>
+    <t>krembo.jpg</t>
+  </si>
+  <si>
+    <t>kube.jpg</t>
+  </si>
+  <si>
+    <t>papaya.jpg</t>
+  </si>
+  <si>
+    <t>pilpel.jpg</t>
+  </si>
+  <si>
+    <t>pita.jpg</t>
+  </si>
+  <si>
+    <t>pitsputseorez.jpg</t>
+  </si>
+  <si>
+    <t>pomela.jpg</t>
+  </si>
+  <si>
+    <t>popcorn.jpg</t>
+  </si>
+  <si>
+    <t>potato.jpg</t>
+  </si>
+  <si>
+    <t>ptitim.jpg</t>
+  </si>
+  <si>
+    <t>rimon.jpg</t>
+  </si>
+  <si>
+    <t>shezif.jpg</t>
+  </si>
+  <si>
+    <t>shtrudel.jpg</t>
+  </si>
+  <si>
+    <t>shum.jpg</t>
+  </si>
+  <si>
+    <t>shumar.jpg</t>
+  </si>
+  <si>
+    <t>tsimukim.jpg</t>
+  </si>
+  <si>
+    <t>tsnon.jpg</t>
+  </si>
+  <si>
+    <t>tsnonit.jpg</t>
+  </si>
+  <si>
+    <t>anavim.png</t>
+  </si>
+  <si>
+    <t>armonim.png</t>
+  </si>
+  <si>
+    <t>puding.png</t>
+  </si>
+  <si>
+    <t>ships.png</t>
+  </si>
+  <si>
+    <t>tsnim.png</t>
+  </si>
+  <si>
+    <t>kubana.png</t>
+  </si>
+  <si>
+    <t>kolorabi.png</t>
+  </si>
+  <si>
+    <t>koktelperot.png</t>
+  </si>
+  <si>
+    <t>ketshop.png</t>
+  </si>
+  <si>
+    <t>kiwi.png</t>
+  </si>
+  <si>
+    <t>kreker.png</t>
+  </si>
+  <si>
+    <t>kashyu.png</t>
+  </si>
+  <si>
+    <t>riba.png</t>
+  </si>
+  <si>
+    <t>shokolad.png</t>
+  </si>
+  <si>
+    <t>shamenet.png</t>
+  </si>
+  <si>
+    <t>shnitsel.png</t>
+  </si>
+  <si>
+    <t>shaked.png</t>
+  </si>
+  <si>
+    <t>shkedemarak.png</t>
+  </si>
+  <si>
+    <t>teena.png</t>
+  </si>
+  <si>
+    <t>tee.png</t>
+  </si>
+  <si>
+    <t>tut.png</t>
+  </si>
+  <si>
+    <t>tiras.png</t>
+  </si>
+  <si>
+    <t>tamar.png</t>
+  </si>
+  <si>
+    <t>orange.png</t>
+  </si>
+  <si>
+    <t>apple.png</t>
+  </si>
+  <si>
+    <t>trufa.png</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1293,6 +1464,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1596,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2605,7 +2777,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -2615,8 +2787,11 @@
       <c r="C81" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E81" s="91" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>89</v>
       </c>
@@ -2626,8 +2801,11 @@
       <c r="C82" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E82" s="91" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>90</v>
       </c>
@@ -2637,8 +2815,11 @@
       <c r="C83" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E83" s="91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>91</v>
       </c>
@@ -2648,8 +2829,11 @@
       <c r="C84" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E84" s="91" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>92</v>
       </c>
@@ -2659,8 +2843,11 @@
       <c r="C85" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E85" s="91" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>93</v>
       </c>
@@ -2670,8 +2857,11 @@
       <c r="C86" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E86" s="91" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>94</v>
       </c>
@@ -2681,8 +2871,11 @@
       <c r="C87" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E87" s="91" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>95</v>
       </c>
@@ -2692,8 +2885,11 @@
       <c r="C88" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E88" s="91" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>96</v>
       </c>
@@ -2703,8 +2899,9 @@
       <c r="C89" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E89" s="91"/>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>97</v>
       </c>
@@ -2714,8 +2911,11 @@
       <c r="C90" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E90" s="91" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>98</v>
       </c>
@@ -2725,8 +2925,11 @@
       <c r="C91" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E91" s="91" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>99</v>
       </c>
@@ -2736,8 +2939,11 @@
       <c r="C92" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E92" s="91" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>100</v>
       </c>
@@ -2747,8 +2953,11 @@
       <c r="C93" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E93" s="91" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>101</v>
       </c>
@@ -2758,8 +2967,11 @@
       <c r="C94" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E94" s="91" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>102</v>
       </c>
@@ -2769,8 +2981,11 @@
       <c r="C95" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E95" s="91" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>103</v>
       </c>
@@ -2780,8 +2995,11 @@
       <c r="C96" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E96" s="91" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>104</v>
       </c>
@@ -2791,8 +3009,11 @@
       <c r="C97" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="91" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
         <v>105</v>
       </c>
@@ -2802,8 +3023,11 @@
       <c r="C98" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E98" s="91" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>106</v>
       </c>
@@ -2813,8 +3037,11 @@
       <c r="C99" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E99" s="91" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="11" t="s">
         <v>107</v>
       </c>
@@ -2824,8 +3051,11 @@
       <c r="C100" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E100" s="91" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
         <v>108</v>
       </c>
@@ -2835,8 +3065,11 @@
       <c r="C101" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E101" s="91" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
         <v>109</v>
       </c>
@@ -2846,8 +3079,11 @@
       <c r="C102" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E102" s="91" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
         <v>111</v>
       </c>
@@ -2857,8 +3093,9 @@
       <c r="C103" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E103" s="91"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="68" t="s">
         <v>157</v>
       </c>
@@ -2868,8 +3105,9 @@
       <c r="C104" s="66" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E104" s="91"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="81" t="s">
         <v>156</v>
       </c>
@@ -2879,8 +3117,9 @@
       <c r="C105" s="82" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E105" s="91"/>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
         <v>112</v>
       </c>
@@ -2890,8 +3129,11 @@
       <c r="C106" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E106" s="91" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="15" t="s">
         <v>113</v>
       </c>
@@ -2901,8 +3143,11 @@
       <c r="C107" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E107" s="91" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="72" t="s">
         <v>114</v>
       </c>
@@ -2912,8 +3157,11 @@
       <c r="C108" s="80" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E108" s="91" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="48" t="s">
         <v>160</v>
       </c>
@@ -2923,8 +3171,11 @@
       <c r="C109" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E109" s="91" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
         <v>115</v>
       </c>
@@ -2934,8 +3185,11 @@
       <c r="C110" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E110" s="91" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
         <v>116</v>
       </c>
@@ -2945,8 +3199,11 @@
       <c r="C111" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E111" s="91" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="72" t="s">
         <v>153</v>
       </c>
@@ -2954,8 +3211,11 @@
         <v>149</v>
       </c>
       <c r="C112" s="77"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E112" s="91" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="74" t="s">
         <v>155</v>
       </c>
@@ -2965,8 +3225,9 @@
       <c r="C113" s="75" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E113" s="91"/>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="73" t="s">
         <v>154</v>
       </c>
@@ -2976,8 +3237,9 @@
       <c r="C114" s="78" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E114" s="91"/>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
         <v>117</v>
       </c>
@@ -2987,8 +3249,11 @@
       <c r="C115" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E115" s="91" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="45" t="s">
         <v>152</v>
       </c>
@@ -2996,8 +3261,9 @@
         <v>18</v>
       </c>
       <c r="C116" s="71"/>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E116" s="91"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
         <v>118</v>
       </c>
@@ -3005,8 +3271,9 @@
         <v>1</v>
       </c>
       <c r="C117" s="49"/>
-    </row>
-    <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E117" s="91"/>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="13" t="s">
         <v>119</v>
       </c>
@@ -3016,8 +3283,11 @@
       <c r="C118" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E118" s="91" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
         <v>120</v>
       </c>
@@ -3027,8 +3297,11 @@
       <c r="C119" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E119" s="91" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="13" t="s">
         <v>121</v>
       </c>
@@ -3038,8 +3311,11 @@
       <c r="C120" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E120" s="91" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
         <v>122</v>
       </c>
@@ -3047,8 +3323,11 @@
         <v>18</v>
       </c>
       <c r="C121" s="49"/>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E121" s="91" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="13" t="s">
         <v>123</v>
       </c>
@@ -3058,8 +3337,11 @@
       <c r="C122" s="14" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E122" s="91" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="68" t="s">
         <v>150</v>
       </c>
@@ -3067,8 +3349,9 @@
         <v>9</v>
       </c>
       <c r="C123" s="66"/>
-    </row>
-    <row r="124" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E123" s="91"/>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="69" t="s">
         <v>151</v>
       </c>
@@ -3076,8 +3359,11 @@
         <v>18</v>
       </c>
       <c r="C124" s="67"/>
-    </row>
-    <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E124" s="91" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
         <v>125</v>
       </c>
@@ -3087,8 +3373,11 @@
       <c r="C125" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E125" s="91" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15" t="s">
         <v>126</v>
       </c>
@@ -3098,8 +3387,11 @@
       <c r="C126" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E126" s="91" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="17" t="s">
         <v>127</v>
       </c>
@@ -3107,8 +3399,11 @@
         <v>18</v>
       </c>
       <c r="C127" s="50"/>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E127" s="91" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="19" t="s">
         <v>128</v>
       </c>
@@ -3118,8 +3413,11 @@
       <c r="C128" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E128" s="91" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="25" t="s">
         <v>129</v>
       </c>
@@ -3127,8 +3425,11 @@
         <v>18</v>
       </c>
       <c r="C129" s="51"/>
-    </row>
-    <row r="130" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E129" s="91" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="52" t="s">
         <v>130</v>
       </c>
@@ -3138,8 +3439,11 @@
       <c r="C130" s="53" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E130" s="91" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="54" t="s">
         <v>131</v>
       </c>
@@ -3149,8 +3453,11 @@
       <c r="C131" s="55" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E131" s="91" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="52" t="s">
         <v>132</v>
       </c>
@@ -3160,8 +3467,11 @@
       <c r="C132" s="53" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E132" s="91" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="54" t="s">
         <v>133</v>
       </c>
@@ -3171,8 +3481,11 @@
       <c r="C133" s="55" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E133" s="91" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="52" t="s">
         <v>134</v>
       </c>
@@ -3182,8 +3495,11 @@
       <c r="C134" s="53" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E134" s="91" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="54" t="s">
         <v>135</v>
       </c>
@@ -3193,8 +3509,11 @@
       <c r="C135" s="55" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E135" s="91" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="52" t="s">
         <v>136</v>
       </c>
@@ -3204,8 +3523,11 @@
       <c r="C136" s="53" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E136" s="91" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="54" t="s">
         <v>137</v>
       </c>
@@ -3215,8 +3537,11 @@
       <c r="C137" s="55" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E137" s="91" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="33" t="s">
         <v>139</v>
       </c>
@@ -3226,8 +3551,11 @@
       <c r="C138" s="34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E138" s="91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="35" t="s">
         <v>140</v>
       </c>
@@ -3237,8 +3565,11 @@
       <c r="C139" s="36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E139" s="91" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="37" t="s">
         <v>141</v>
       </c>
@@ -3248,8 +3579,11 @@
       <c r="C140" s="38" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E140" s="91" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="35" t="s">
         <v>142</v>
       </c>
@@ -3259,8 +3593,11 @@
       <c r="C141" s="36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E141" s="91" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="37" t="s">
         <v>143</v>
       </c>
@@ -3270,8 +3607,11 @@
       <c r="C142" s="38" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E142" s="91" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="35" t="s">
         <v>144</v>
       </c>
@@ -3281,8 +3621,11 @@
       <c r="C143" s="36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E143" s="91" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="37" t="s">
         <v>145</v>
       </c>
@@ -3292,8 +3635,11 @@
       <c r="C144" s="38" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E144" s="91" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="35" t="s">
         <v>146</v>
       </c>
@@ -3303,8 +3649,11 @@
       <c r="C145" s="36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="91" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="60" t="s">
         <v>147</v>
       </c>
@@ -3312,8 +3661,11 @@
         <v>149</v>
       </c>
       <c r="C146" s="63"/>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E146" s="91" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="61" t="s">
         <v>148</v>
       </c>
@@ -3322,7 +3674,7 @@
       </c>
       <c r="C147" s="64"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="90" t="s">
         <v>204</v>
       </c>
@@ -3330,7 +3682,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="90" t="s">
         <v>206</v>
       </c>
@@ -3338,7 +3690,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="90" t="s">
         <v>209</v>
       </c>
@@ -3346,7 +3698,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="90" t="s">
         <v>210</v>
       </c>

</xml_diff>

<commit_message>
fix some values in ds table
</commit_message>
<xml_diff>
--- a/DataSet.xlsx
+++ b/DataSet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Yair_Projects\PythonProjects\guess_the_bless\guess_the_bless\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="266">
   <si>
     <t>אבוקדו</t>
   </si>
@@ -285,9 +290,6 @@
     <t>פיסטוק</t>
   </si>
   <si>
-    <t>פיצה על מצה</t>
-  </si>
-  <si>
     <t>פיתה</t>
   </si>
   <si>
@@ -420,9 +422,6 @@
     <t>תרופה בלי טעם</t>
   </si>
   <si>
-    <t>תרופה טעימה</t>
-  </si>
-  <si>
     <t>לא מברך</t>
   </si>
   <si>
@@ -817,17 +816,20 @@
   </si>
   <si>
     <t xml:space="preserve">מזונות </t>
+  </si>
+  <si>
+    <t>פיצה על מצה תוך כדי חג הפסח</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1160,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1321,9 +1323,6 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1336,16 +1335,10 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1437,12 +1430,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1484,7 +1480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1517,9 +1513,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1552,6 +1565,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1728,21 +1758,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1753,10 +1783,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1767,24 +1797,24 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1795,10 +1825,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1809,7 +1839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1820,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1834,10 +1864,10 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1848,10 +1878,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1862,7 +1892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -1873,7 +1903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1884,10 +1914,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1898,7 +1928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1909,10 +1939,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1923,7 +1953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1934,10 +1964,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>20</v>
       </c>
@@ -1948,12 +1978,12 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>9</v>
@@ -1962,10 +1992,10 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
@@ -1976,10 +2006,10 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>22</v>
       </c>
@@ -1990,10 +2020,10 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
@@ -2004,10 +2034,10 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
@@ -2018,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
@@ -2032,10 +2062,10 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
@@ -2046,10 +2076,10 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>27</v>
       </c>
@@ -2060,10 +2090,10 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
@@ -2074,7 +2104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>29</v>
       </c>
@@ -2085,10 +2115,10 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>30</v>
       </c>
@@ -2099,10 +2129,10 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>31</v>
       </c>
@@ -2113,7 +2143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>32</v>
       </c>
@@ -2124,10 +2154,10 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>33</v>
       </c>
@@ -2138,7 +2168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>34</v>
       </c>
@@ -2149,10 +2179,10 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>35</v>
       </c>
@@ -2163,9 +2193,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>18</v>
@@ -2174,7 +2204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
@@ -2185,12 +2215,12 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>4</v>
@@ -2199,10 +2229,10 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>37</v>
       </c>
@@ -2213,10 +2243,10 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>38</v>
       </c>
@@ -2227,10 +2257,10 @@
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>39</v>
       </c>
@@ -2241,10 +2271,10 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>40</v>
       </c>
@@ -2255,10 +2285,10 @@
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>41</v>
       </c>
@@ -2269,10 +2299,10 @@
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>42</v>
       </c>
@@ -2283,7 +2313,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>44</v>
       </c>
@@ -2294,7 +2324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>45</v>
       </c>
@@ -2305,10 +2335,10 @@
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -2319,9 +2349,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>18</v>
@@ -2330,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>49</v>
       </c>
@@ -2341,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -2352,10 +2382,10 @@
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -2366,10 +2396,10 @@
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -2380,7 +2410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>53</v>
       </c>
@@ -2391,7 +2421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>54</v>
       </c>
@@ -2402,7 +2432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>55</v>
       </c>
@@ -2413,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>56</v>
       </c>
@@ -2424,10 +2454,10 @@
         <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>59</v>
       </c>
@@ -2438,7 +2468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>60</v>
       </c>
@@ -2449,7 +2479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>61</v>
       </c>
@@ -2460,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>62</v>
       </c>
@@ -2471,7 +2501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
         <v>63</v>
       </c>
@@ -2482,10 +2512,10 @@
         <v>48</v>
       </c>
       <c r="E58" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
         <v>64</v>
       </c>
@@ -2496,23 +2526,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="81" t="s">
+      <c r="C60" s="78" t="s">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>18</v>
@@ -2521,7 +2551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>66</v>
       </c>
@@ -2532,7 +2562,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
@@ -2543,7 +2573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>69</v>
       </c>
@@ -2554,7 +2584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>70</v>
       </c>
@@ -2565,10 +2595,10 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>71</v>
       </c>
@@ -2579,7 +2609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>72</v>
       </c>
@@ -2588,29 +2618,29 @@
       </c>
       <c r="C67" s="39"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="B68" s="84" t="s">
+    <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A68" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="83" t="s">
-        <v>144</v>
-      </c>
-      <c r="B69" s="86" t="s">
+      <c r="C68" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A69" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="87" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>73</v>
       </c>
@@ -2621,7 +2651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>74</v>
       </c>
@@ -2632,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>75</v>
       </c>
@@ -2643,10 +2673,10 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>76</v>
       </c>
@@ -2657,7 +2687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>77</v>
       </c>
@@ -2666,7 +2696,7 @@
       </c>
       <c r="C74" s="40"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
         <v>78</v>
       </c>
@@ -2677,12 +2707,12 @@
         <v>11</v>
       </c>
       <c r="E75" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>4</v>
@@ -2691,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>79</v>
       </c>
@@ -2702,21 +2732,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C78" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>81</v>
       </c>
@@ -2727,10 +2757,10 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
@@ -2740,11 +2770,11 @@
       <c r="C80" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E80" s="89" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E80" s="86" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>83</v>
       </c>
@@ -2754,13 +2784,13 @@
       <c r="C81" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E81" s="89" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E81" s="86" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>18</v>
@@ -2768,11 +2798,11 @@
       <c r="C82" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E82" s="89" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E82" s="86" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>84</v>
       </c>
@@ -2782,11 +2812,11 @@
       <c r="C83" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="89" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E83" s="86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
@@ -2796,11 +2826,11 @@
       <c r="C84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E84" s="89" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E84" s="86" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>86</v>
       </c>
@@ -2810,11 +2840,11 @@
       <c r="C85" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E85" s="89" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E85" s="86" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
@@ -2824,11 +2854,11 @@
       <c r="C86" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E86" s="89" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E86" s="86" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>88</v>
       </c>
@@ -2838,13 +2868,13 @@
       <c r="C87" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E87" s="89" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E87" s="86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>89</v>
+        <v>265</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>47</v>
@@ -2852,11 +2882,11 @@
       <c r="C88" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E88" s="89"/>
-    </row>
-    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E88" s="86"/>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>47</v>
@@ -2864,13 +2894,13 @@
       <c r="C89" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E89" s="89" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E89" s="86" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>4</v>
@@ -2878,13 +2908,13 @@
       <c r="C90" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E90" s="89" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E90" s="86" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>9</v>
@@ -2892,13 +2922,13 @@
       <c r="C91" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E91" s="89" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E91" s="86" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>4</v>
@@ -2906,13 +2936,13 @@
       <c r="C92" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E92" s="89" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E92" s="86" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
@@ -2920,13 +2950,13 @@
       <c r="C93" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E93" s="89" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E93" s="86" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>1</v>
@@ -2934,13 +2964,13 @@
       <c r="C94" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E94" s="89" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E94" s="86" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>4</v>
@@ -2948,13 +2978,13 @@
       <c r="C95" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E95" s="89" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E95" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>4</v>
@@ -2962,13 +2992,13 @@
       <c r="C96" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E96" s="89" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E96" s="86" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>4</v>
@@ -2976,13 +3006,13 @@
       <c r="C97" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E97" s="89" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="86" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>47</v>
@@ -2990,13 +3020,13 @@
       <c r="C98" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E98" s="89" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E98" s="86" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B99" s="12" t="s">
         <v>18</v>
@@ -3004,13 +3034,13 @@
       <c r="C99" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E99" s="89" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E99" s="86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>9</v>
@@ -3018,27 +3048,27 @@
       <c r="C100" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E100" s="89" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E100" s="86" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C101" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E101" s="89" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E101" s="86" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>9</v>
@@ -3046,35 +3076,35 @@
       <c r="C102" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E102" s="89"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="B103" s="63" t="s">
+      <c r="E102" s="86"/>
+    </row>
+    <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A103" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B103" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C103" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="E103" s="89"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="79" t="s">
-        <v>142</v>
+      <c r="C103" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E103" s="86"/>
+    </row>
+    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A104" s="76" t="s">
+        <v>140</v>
       </c>
       <c r="B104" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="E104" s="89"/>
-    </row>
-    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="86"/>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>4</v>
@@ -3082,13 +3112,13 @@
       <c r="C105" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="89" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E105" s="86" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" s="16" t="s">
         <v>1</v>
@@ -3096,55 +3126,55 @@
       <c r="C106" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E106" s="89" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="70" t="s">
+      <c r="E106" s="86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A107" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="B107" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="E107" s="86" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E108" s="86" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E109" s="86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="B107" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="E107" s="89" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="B108" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C108" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E108" s="89" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="B109" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C109" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E109" s="89" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="15" t="s">
-        <v>106</v>
       </c>
       <c r="B110" s="16" t="s">
         <v>1</v>
@@ -3152,49 +3182,49 @@
       <c r="C110" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="89" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="70" t="s">
+      <c r="E110" s="86" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A111" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="B111" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="C111" s="72"/>
+      <c r="E111" s="86" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A112" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="B111" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="C111" s="75"/>
-      <c r="E111" s="89" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="72" t="s">
-        <v>141</v>
-      </c>
       <c r="B112" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C112" s="73" t="s">
-        <v>2</v>
-      </c>
-      <c r="E112" s="89"/>
-    </row>
-    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="71" t="s">
-        <v>140</v>
+      <c r="C112" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E112" s="86"/>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="68" t="s">
+        <v>138</v>
       </c>
       <c r="B113" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C113" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="E113" s="89"/>
-    </row>
-    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E113" s="86"/>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B114" s="16" t="s">
         <v>4</v>
@@ -3202,33 +3232,33 @@
       <c r="C114" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E114" s="89" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="86" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="B115" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="C115" s="69"/>
-      <c r="E115" s="89"/>
-    </row>
-    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="B115" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C115" s="66"/>
+      <c r="E115" s="86"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B116" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C116" s="47"/>
-      <c r="E116" s="89"/>
-    </row>
-    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E116" s="86"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B117" s="14" t="s">
         <v>1</v>
@@ -3236,13 +3266,13 @@
       <c r="C117" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="89" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E117" s="86" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B118" s="16" t="s">
         <v>9</v>
@@ -3250,13 +3280,13 @@
       <c r="C118" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E118" s="89" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E118" s="86" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B119" s="14" t="s">
         <v>18</v>
@@ -3264,61 +3294,61 @@
       <c r="C119" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E119" s="89" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E119" s="86" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C120" s="47"/>
+      <c r="E120" s="86" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C121" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B120" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C120" s="47"/>
-      <c r="E120" s="89" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C121" s="14" t="s">
+      <c r="E121" s="86" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A122" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B122" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="61"/>
+      <c r="E122" s="86"/>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="64" t="s">
+        <v>135</v>
+      </c>
+      <c r="B123" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C123" s="62"/>
+      <c r="E123" s="86" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="E121" s="89" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="66" t="s">
-        <v>136</v>
-      </c>
-      <c r="B122" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C122" s="64"/>
-      <c r="E122" s="89"/>
-    </row>
-    <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="B123" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C123" s="65"/>
-      <c r="E123" s="89" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="B124" s="14" t="s">
         <v>9</v>
@@ -3326,13 +3356,13 @@
       <c r="C124" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E124" s="89" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E124" s="86" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B125" s="16" t="s">
         <v>1</v>
@@ -3340,25 +3370,25 @@
       <c r="C125" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E125" s="89" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E125" s="86" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B126" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" s="48"/>
+      <c r="E126" s="86" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="B126" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C126" s="48"/>
-      <c r="E126" s="89" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="B127" s="20" t="s">
         <v>1</v>
@@ -3366,53 +3396,53 @@
       <c r="C127" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E127" s="89" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E127" s="86" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="25" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B128" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C128" s="49"/>
-      <c r="E128" s="89" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E128" s="86" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C129" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="86" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="B129" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C129" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="89" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="52" t="s">
+      <c r="B130" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C130" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E130" s="86" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="50" t="s">
         <v>118</v>
-      </c>
-      <c r="B130" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="C130" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="E130" s="89" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="50" t="s">
-        <v>119</v>
       </c>
       <c r="B131" s="51" t="s">
         <v>1</v>
@@ -3420,13 +3450,13 @@
       <c r="C131" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E131" s="89" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E131" s="86" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B132" s="53" t="s">
         <v>9</v>
@@ -3434,41 +3464,41 @@
       <c r="C132" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="E132" s="89" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E132" s="86" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B133" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C133" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E133" s="86" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="B133" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C133" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="E133" s="89" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="52" t="s">
+      <c r="B134" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C134" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E134" s="86" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="50" t="s">
         <v>122</v>
-      </c>
-      <c r="B134" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="C134" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="E134" s="89" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="50" t="s">
-        <v>123</v>
       </c>
       <c r="B135" s="51" t="s">
         <v>1</v>
@@ -3476,27 +3506,27 @@
       <c r="C135" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E135" s="89" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E135" s="86" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B136" s="53" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C136" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="E136" s="89" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E136" s="86" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B137" s="32" t="s">
         <v>1</v>
@@ -3504,27 +3534,27 @@
       <c r="C137" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E137" s="89" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E137" s="86" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B138" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C138" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E138" s="86" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="35" t="s">
         <v>126</v>
-      </c>
-      <c r="B138" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C138" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E138" s="89" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="35" t="s">
-        <v>127</v>
       </c>
       <c r="B139" s="36" t="s">
         <v>4</v>
@@ -3532,13 +3562,13 @@
       <c r="C139" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E139" s="89" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E139" s="86" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B140" s="34" t="s">
         <v>4</v>
@@ -3546,13 +3576,13 @@
       <c r="C140" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E140" s="89" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E140" s="86" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B141" s="36" t="s">
         <v>1</v>
@@ -3560,13 +3590,13 @@
       <c r="C141" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E141" s="89" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E141" s="86" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B142" s="34" t="s">
         <v>1</v>
@@ -3574,13 +3604,13 @@
       <c r="C142" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E142" s="89" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E142" s="86" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B143" s="36" t="s">
         <v>1</v>
@@ -3588,13 +3618,13 @@
       <c r="C143" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E143" s="89" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E143" s="86" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B144" s="34" t="s">
         <v>4</v>
@@ -3602,61 +3632,52 @@
       <c r="C144" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E144" s="89" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="58" t="s">
+      <c r="E144" s="86" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A145" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="B145" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B145" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="C145" s="61"/>
-      <c r="E145" s="89" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="B146" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C146" s="62"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="88" t="s">
+      <c r="C145" s="59"/>
+      <c r="E145" s="86" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A146" s="85" t="s">
+        <v>188</v>
+      </c>
+      <c r="D146" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A147" s="85" t="s">
         <v>190</v>
       </c>
       <c r="D147" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="88" t="s">
+    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A148" s="85" t="s">
+        <v>193</v>
+      </c>
+      <c r="D148" t="s">
         <v>192</v>
       </c>
-      <c r="D148" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="88" t="s">
+    </row>
+    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A149" s="85" t="s">
+        <v>194</v>
+      </c>
+      <c r="D149" t="s">
         <v>195</v>
-      </c>
-      <c r="D149" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="88" t="s">
-        <v>196</v>
-      </c>
-      <c r="D150" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +3692,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3683,7 +3704,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>